<commit_message>
Megan: paper 11 rubric and report submission
information about paper 11 inputed to both the rubric and report.
</commit_message>
<xml_diff>
--- a/Cols_draft_M5.xlsx
+++ b/Cols_draft_M5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganng/Documents/GitHub/QLSC600D2_2025_M5A1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B48DB5-F3BA-FC46-BF3C-9E3857853611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE0DF80-727D-0F45-BF8F-B37EF64B822B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{36676770-CB25-F949-8228-BA136C80F5EB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>Link to article</t>
   </si>
@@ -208,7 +208,19 @@
     <t>Organizing principles of astrocytic nanoarchitecture in the mouse cerebral cortex</t>
   </si>
   <si>
-    <t xml:space="preserve">https://pubmed.ncbi.nlm.nih.gov/36805126/ </t>
+    <t>Cardiomyocyte orientation recovery at micrometer scale reveals long‐axis fiber continuum in heart walls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1016/j.cub.2023.01.043 </t>
+  </si>
+  <si>
+    <t>https://doi.org/10.15252/embj.2022113288</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was an easy read. Methodology and materials clearly described. Great "key resources" table.  However, a request must be made to the "lead contact" to access datasets generated. This may be inconvenient and/or time consuming. </t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -949,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037553EA-793E-E147-BDF6-0B4A3FE59E4A}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="94" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1290,15 +1302,8 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="6">
-        <v>2023</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>44</v>
-      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
       <c r="E12" s="18" t="s">
         <v>35</v>
       </c>
@@ -1316,7 +1321,6 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="18" t="s">
@@ -1356,29 +1360,57 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="B15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2023</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>45</v>
+      </c>
       <c r="E15" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
+      <c r="F15" s="6">
+        <v>4</v>
+      </c>
+      <c r="G15" s="6">
+        <v>5</v>
+      </c>
+      <c r="H15" s="6">
+        <v>5</v>
+      </c>
+      <c r="I15" s="6">
+        <v>5</v>
+      </c>
+      <c r="J15" s="6">
+        <v>5</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="1:13" s="1" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2023</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="E16" s="6" t="s">
         <v>42</v>
       </c>
@@ -2094,9 +2126,10 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{76023512-4294-824B-9C48-0092BD200719}"/>
-    <hyperlink ref="D12" r:id="rId2" xr:uid="{F5278718-A4B4-4240-985E-B0483DC8FE28}"/>
+    <hyperlink ref="D15" r:id="rId2" xr:uid="{F5278718-A4B4-4240-985E-B0483DC8FE28}"/>
     <hyperlink ref="D10" r:id="rId3" xr:uid="{D9D5E1C5-2E77-904A-AA9E-B48D428046B2}"/>
     <hyperlink ref="D11" r:id="rId4" xr:uid="{05674F12-7BCD-F047-B51E-2A47BBB4405F}"/>
+    <hyperlink ref="D16" r:id="rId5" xr:uid="{0B33E01C-4B02-5242-BC18-EC2B0587BFAC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Megan: paper 12 information upload to rubric and report
</commit_message>
<xml_diff>
--- a/Cols_draft_M5.xlsx
+++ b/Cols_draft_M5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganng/Documents/GitHub/QLSC600D2_2025_M5A1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE0DF80-727D-0F45-BF8F-B37EF64B822B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BEBB62-257E-5645-9734-8EACBDF00F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{36676770-CB25-F949-8228-BA136C80F5EB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>Link to article</t>
   </si>
@@ -208,19 +208,22 @@
     <t>Organizing principles of astrocytic nanoarchitecture in the mouse cerebral cortex</t>
   </si>
   <si>
-    <t>Cardiomyocyte orientation recovery at micrometer scale reveals long‐axis fiber continuum in heart walls</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://doi.org/10.1016/j.cub.2023.01.043 </t>
   </si>
   <si>
-    <t>https://doi.org/10.15252/embj.2022113288</t>
-  </si>
-  <si>
     <t xml:space="preserve">Was an easy read. Methodology and materials clearly described. Great "key resources" table.  However, a request must be made to the "lead contact" to access datasets generated. This may be inconvenient and/or time consuming. </t>
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/jnr.24386</t>
+  </si>
+  <si>
+    <t>Glycogen distribution in mouse hippocampus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qualitative study with minimal detail and inaccesible equipment. </t>
   </si>
 </sst>
 </file>
@@ -961,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037553EA-793E-E147-BDF6-0B4A3FE59E4A}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="94" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="94" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1367,7 +1370,7 @@
         <v>2023</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>42</v>
@@ -1388,13 +1391,13 @@
         <v>5</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="1" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
@@ -1403,25 +1406,41 @@
         <v>12</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C16" s="6">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
+      <c r="F16" s="6">
+        <v>1</v>
+      </c>
+      <c r="G16" s="6">
+        <v>3</v>
+      </c>
+      <c r="H16" s="6">
+        <v>2</v>
+      </c>
+      <c r="I16" s="6">
+        <v>2</v>
+      </c>
+      <c r="J16" s="6">
+        <v>2</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="17" spans="1:13" s="1" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
@@ -2129,7 +2148,6 @@
     <hyperlink ref="D15" r:id="rId2" xr:uid="{F5278718-A4B4-4240-985E-B0483DC8FE28}"/>
     <hyperlink ref="D10" r:id="rId3" xr:uid="{D9D5E1C5-2E77-904A-AA9E-B48D428046B2}"/>
     <hyperlink ref="D11" r:id="rId4" xr:uid="{05674F12-7BCD-F047-B51E-2A47BBB4405F}"/>
-    <hyperlink ref="D16" r:id="rId5" xr:uid="{0B33E01C-4B02-5242-BC18-EC2B0587BFAC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Megan: adding publication year info
</commit_message>
<xml_diff>
--- a/Cols_draft_M5.xlsx
+++ b/Cols_draft_M5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganng/Documents/GitHub/QLSC600D2_2025_M5A1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BEBB62-257E-5645-9734-8EACBDF00F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9F50C4-B3A0-4D42-B5FD-508D56FE9F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{36676770-CB25-F949-8228-BA136C80F5EB}"/>
   </bookViews>
@@ -964,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037553EA-793E-E147-BDF6-0B4A3FE59E4A}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="94" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="94" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1409,7 +1409,7 @@
         <v>48</v>
       </c>
       <c r="C16" s="6">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>47</v>

</xml_diff>